<commit_message>
Changed the logo and added a new job.
</commit_message>
<xml_diff>
--- a/Jobs/HomeJobs.xlsx
+++ b/Jobs/HomeJobs.xlsx
@@ -16,14 +16,11 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="256" uniqueCount="71">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="251" uniqueCount="80">
   <si>
     <t>Gr. Noida</t>
   </si>
   <si>
-    <t>Gurugaon</t>
-  </si>
-  <si>
     <t>Faridabad</t>
   </si>
   <si>
@@ -147,9 +144,6 @@
     <t>Canteen Free</t>
   </si>
   <si>
-    <t>Home Job2 (INDIA) PVT. LTD.</t>
-  </si>
-  <si>
     <t>Home Job3 (INDIA) PVT. LTD.</t>
   </si>
   <si>
@@ -229,6 +223,39 @@
   </si>
   <si>
     <t>पहले आओ | पहले पाओ ||</t>
+  </si>
+  <si>
+    <t>Itel MNC Company</t>
+  </si>
+  <si>
+    <t>Noida Sector 63</t>
+  </si>
+  <si>
+    <t>इंटरव्यू पता :- ARK Workforce Plot Number – 246 Block – G Sector-63 Noida</t>
+  </si>
+  <si>
+    <t xml:space="preserve">इंटरव्यू टाइम :- 11 बजे तक </t>
+  </si>
+  <si>
+    <t>इंटरव्यू की तारीख: 04/04/2025</t>
+  </si>
+  <si>
+    <t>Contact person: Ankit -8477873797, Vishan – 9315473717</t>
+  </si>
+  <si>
+    <t>Qualification:-10th 12th graduate ITI or Diploma</t>
+  </si>
+  <si>
+    <t>Salary: 11000 Rs in hand</t>
+  </si>
+  <si>
+    <t>Total Vacancy :- 100(Only Boys)</t>
+  </si>
+  <si>
+    <t>अतिरिक्त लाभ: attendance award: 1000 Rs, Night Alowance 50  Rs Per Night, Overtime: 100 Rs Per Hour, Lunch_Dinner_Free</t>
+  </si>
+  <si>
+    <t>NOTE-: एक साल के बाद भारत सरकार के द्वारा APPPRENTICESHIP का CERTIFICATE मिलता है जिसको कही भी आप एक्सपेरिएंस सर्टिफिकेट की तरह उपयोग कर सकते है.</t>
   </si>
 </sst>
 </file>
@@ -583,8 +610,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X14"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="R2" sqref="R2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="U3" sqref="U3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -596,76 +623,76 @@
   <sheetData>
     <row r="1" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A1" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="C1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="B1" s="2" t="s">
+      <c r="D1" s="2" t="s">
+        <v>6</v>
+      </c>
+      <c r="E1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="C1" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>7</v>
-      </c>
-      <c r="E1" s="1" t="s">
+      <c r="F1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="G1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="H1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="H1" s="1" t="s">
+      <c r="I1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="I1" s="1" t="s">
+      <c r="J1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="J1" s="1" t="s">
+      <c r="K1" s="1" t="s">
         <v>14</v>
       </c>
-      <c r="K1" s="1" t="s">
+      <c r="L1" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="L1" s="1" t="s">
+      <c r="M1" s="1" t="s">
         <v>16</v>
       </c>
-      <c r="M1" s="1" t="s">
+      <c r="N1" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="N1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>18</v>
       </c>
-      <c r="O1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>19</v>
       </c>
-      <c r="P1" s="1" t="s">
+      <c r="Q1" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="Q1" s="1" t="s">
+      <c r="R1" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="R1" s="1" t="s">
+      <c r="S1" s="1" t="s">
         <v>22</v>
       </c>
-      <c r="S1" s="1" t="s">
+      <c r="T1" t="s">
         <v>23</v>
       </c>
-      <c r="T1" t="s">
+      <c r="U1" t="s">
         <v>24</v>
       </c>
-      <c r="U1" t="s">
+      <c r="V1" t="s">
         <v>25</v>
       </c>
-      <c r="V1" t="s">
+      <c r="W1" t="s">
         <v>26</v>
       </c>
-      <c r="W1" t="s">
+      <c r="X1" t="s">
         <v>27</v>
-      </c>
-      <c r="X1" t="s">
-        <v>28</v>
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
@@ -673,55 +700,55 @@
         <v>1</v>
       </c>
       <c r="B2" t="s">
+        <v>53</v>
+      </c>
+      <c r="C2" t="s">
+        <v>54</v>
+      </c>
+      <c r="D2" t="s">
+        <v>62</v>
+      </c>
+      <c r="E2" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" t="s">
+        <v>61</v>
+      </c>
+      <c r="G2" t="s">
+        <v>56</v>
+      </c>
+      <c r="H2" t="s">
+        <v>57</v>
+      </c>
+      <c r="I2" t="s">
+        <v>58</v>
+      </c>
+      <c r="J2" t="s">
+        <v>59</v>
+      </c>
+      <c r="K2" t="s">
         <v>55</v>
       </c>
-      <c r="C2" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="L2" t="s">
+        <v>63</v>
+      </c>
+      <c r="M2" t="s">
         <v>64</v>
       </c>
-      <c r="E2" t="s">
-        <v>64</v>
-      </c>
-      <c r="F2" t="s">
-        <v>63</v>
-      </c>
-      <c r="G2" t="s">
-        <v>58</v>
-      </c>
-      <c r="H2" t="s">
-        <v>59</v>
-      </c>
-      <c r="I2" t="s">
+      <c r="N2" t="s">
+        <v>65</v>
+      </c>
+      <c r="O2" t="s">
+        <v>67</v>
+      </c>
+      <c r="P2" t="s">
+        <v>66</v>
+      </c>
+      <c r="Q2" t="s">
         <v>60</v>
       </c>
-      <c r="J2" t="s">
-        <v>61</v>
-      </c>
-      <c r="K2" t="s">
-        <v>57</v>
-      </c>
-      <c r="L2" t="s">
-        <v>65</v>
-      </c>
-      <c r="M2" t="s">
-        <v>66</v>
-      </c>
-      <c r="N2" t="s">
-        <v>67</v>
-      </c>
-      <c r="O2" t="s">
-        <v>69</v>
-      </c>
-      <c r="P2" t="s">
+      <c r="R2" t="s">
         <v>68</v>
-      </c>
-      <c r="Q2" t="s">
-        <v>62</v>
-      </c>
-      <c r="R2" t="s">
-        <v>70</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
@@ -729,58 +756,43 @@
         <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>43</v>
+        <v>69</v>
       </c>
       <c r="C3" t="s">
-        <v>1</v>
+        <v>70</v>
       </c>
       <c r="D3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E3" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F3" t="s">
-        <v>29</v>
+        <v>71</v>
       </c>
       <c r="G3" t="s">
-        <v>30</v>
+        <v>73</v>
       </c>
       <c r="H3" t="s">
-        <v>31</v>
+        <v>72</v>
       </c>
       <c r="I3" t="s">
-        <v>32</v>
+        <v>74</v>
       </c>
       <c r="J3" t="s">
-        <v>33</v>
+        <v>75</v>
       </c>
       <c r="K3" t="s">
-        <v>34</v>
+        <v>76</v>
       </c>
       <c r="L3" t="s">
-        <v>35</v>
+        <v>77</v>
       </c>
       <c r="M3" t="s">
-        <v>36</v>
+        <v>78</v>
       </c>
       <c r="N3" t="s">
-        <v>37</v>
-      </c>
-      <c r="O3" t="s">
-        <v>38</v>
-      </c>
-      <c r="P3" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q3" t="s">
-        <v>39</v>
-      </c>
-      <c r="R3" t="s">
-        <v>40</v>
-      </c>
-      <c r="S3" t="s">
-        <v>41</v>
+        <v>79</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
@@ -788,58 +800,58 @@
         <v>3</v>
       </c>
       <c r="B4" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E4" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F4" t="s">
+        <v>28</v>
+      </c>
+      <c r="G4" t="s">
         <v>29</v>
       </c>
-      <c r="G4" t="s">
+      <c r="H4" t="s">
         <v>30</v>
       </c>
-      <c r="H4" t="s">
+      <c r="I4" t="s">
         <v>31</v>
       </c>
-      <c r="I4" t="s">
+      <c r="J4" t="s">
         <v>32</v>
       </c>
-      <c r="J4" t="s">
+      <c r="K4" t="s">
         <v>33</v>
       </c>
-      <c r="K4" t="s">
+      <c r="L4" t="s">
         <v>34</v>
       </c>
-      <c r="L4" t="s">
+      <c r="M4" t="s">
         <v>35</v>
       </c>
-      <c r="M4" t="s">
+      <c r="N4" t="s">
         <v>36</v>
       </c>
-      <c r="N4" t="s">
+      <c r="O4" t="s">
         <v>37</v>
       </c>
-      <c r="O4" t="s">
+      <c r="P4" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q4" t="s">
         <v>38</v>
       </c>
-      <c r="P4" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q4" t="s">
+      <c r="R4" t="s">
         <v>39</v>
       </c>
-      <c r="R4" t="s">
+      <c r="S4" t="s">
         <v>40</v>
-      </c>
-      <c r="S4" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
@@ -847,58 +859,58 @@
         <v>4</v>
       </c>
       <c r="B5" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C5" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="D5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E5" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F5" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" t="s">
         <v>29</v>
       </c>
-      <c r="G5" t="s">
+      <c r="H5" t="s">
         <v>30</v>
       </c>
-      <c r="H5" t="s">
+      <c r="I5" t="s">
         <v>31</v>
       </c>
-      <c r="I5" t="s">
+      <c r="J5" t="s">
         <v>32</v>
       </c>
-      <c r="J5" t="s">
+      <c r="K5" t="s">
         <v>33</v>
       </c>
-      <c r="K5" t="s">
+      <c r="L5" t="s">
         <v>34</v>
       </c>
-      <c r="L5" t="s">
+      <c r="M5" t="s">
         <v>35</v>
       </c>
-      <c r="M5" t="s">
+      <c r="N5" t="s">
         <v>36</v>
       </c>
-      <c r="N5" t="s">
+      <c r="O5" t="s">
         <v>37</v>
       </c>
-      <c r="O5" t="s">
+      <c r="P5" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q5" t="s">
         <v>38</v>
       </c>
-      <c r="P5" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q5" t="s">
+      <c r="R5" t="s">
         <v>39</v>
       </c>
-      <c r="R5" t="s">
+      <c r="S5" t="s">
         <v>40</v>
-      </c>
-      <c r="S5" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
@@ -906,58 +918,58 @@
         <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C6" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="D6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E6" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F6" t="s">
+        <v>28</v>
+      </c>
+      <c r="G6" t="s">
         <v>29</v>
       </c>
-      <c r="G6" t="s">
+      <c r="H6" t="s">
         <v>30</v>
       </c>
-      <c r="H6" t="s">
+      <c r="I6" t="s">
         <v>31</v>
       </c>
-      <c r="I6" t="s">
+      <c r="J6" t="s">
         <v>32</v>
       </c>
-      <c r="J6" t="s">
+      <c r="K6" t="s">
         <v>33</v>
       </c>
-      <c r="K6" t="s">
+      <c r="L6" t="s">
         <v>34</v>
       </c>
-      <c r="L6" t="s">
+      <c r="M6" t="s">
         <v>35</v>
       </c>
-      <c r="M6" t="s">
+      <c r="N6" t="s">
         <v>36</v>
       </c>
-      <c r="N6" t="s">
+      <c r="O6" t="s">
         <v>37</v>
       </c>
-      <c r="O6" t="s">
+      <c r="P6" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q6" t="s">
         <v>38</v>
       </c>
-      <c r="P6" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q6" t="s">
+      <c r="R6" t="s">
         <v>39</v>
       </c>
-      <c r="R6" t="s">
+      <c r="S6" t="s">
         <v>40</v>
-      </c>
-      <c r="S6" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
@@ -965,58 +977,58 @@
         <v>6</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C7" t="s">
         <v>0</v>
       </c>
       <c r="D7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E7" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F7" t="s">
+        <v>28</v>
+      </c>
+      <c r="G7" t="s">
         <v>29</v>
       </c>
-      <c r="G7" t="s">
+      <c r="H7" t="s">
         <v>30</v>
       </c>
-      <c r="H7" t="s">
+      <c r="I7" t="s">
         <v>31</v>
       </c>
-      <c r="I7" t="s">
+      <c r="J7" t="s">
         <v>32</v>
       </c>
-      <c r="J7" t="s">
+      <c r="K7" t="s">
         <v>33</v>
       </c>
-      <c r="K7" t="s">
+      <c r="L7" t="s">
         <v>34</v>
       </c>
-      <c r="L7" t="s">
+      <c r="M7" t="s">
         <v>35</v>
       </c>
-      <c r="M7" t="s">
+      <c r="N7" t="s">
         <v>36</v>
       </c>
-      <c r="N7" t="s">
+      <c r="O7" t="s">
         <v>37</v>
       </c>
-      <c r="O7" t="s">
+      <c r="P7" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q7" t="s">
         <v>38</v>
       </c>
-      <c r="P7" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q7" t="s">
+      <c r="R7" t="s">
         <v>39</v>
       </c>
-      <c r="R7" t="s">
+      <c r="S7" t="s">
         <v>40</v>
-      </c>
-      <c r="S7" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
@@ -1024,58 +1036,58 @@
         <v>7</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="C8" t="s">
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E8" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F8" t="s">
+        <v>28</v>
+      </c>
+      <c r="G8" t="s">
         <v>29</v>
       </c>
-      <c r="G8" t="s">
+      <c r="H8" t="s">
         <v>30</v>
       </c>
-      <c r="H8" t="s">
+      <c r="I8" t="s">
         <v>31</v>
       </c>
-      <c r="I8" t="s">
+      <c r="J8" t="s">
         <v>32</v>
       </c>
-      <c r="J8" t="s">
+      <c r="K8" t="s">
         <v>33</v>
       </c>
-      <c r="K8" t="s">
+      <c r="L8" t="s">
         <v>34</v>
       </c>
-      <c r="L8" t="s">
+      <c r="M8" t="s">
         <v>35</v>
       </c>
-      <c r="M8" t="s">
+      <c r="N8" t="s">
         <v>36</v>
       </c>
-      <c r="N8" t="s">
+      <c r="O8" t="s">
         <v>37</v>
       </c>
-      <c r="O8" t="s">
+      <c r="P8" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q8" t="s">
         <v>38</v>
       </c>
-      <c r="P8" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q8" t="s">
+      <c r="R8" t="s">
         <v>39</v>
       </c>
-      <c r="R8" t="s">
+      <c r="S8" t="s">
         <v>40</v>
-      </c>
-      <c r="S8" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
@@ -1083,58 +1095,58 @@
         <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C9" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E9" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
+        <v>28</v>
+      </c>
+      <c r="G9" t="s">
         <v>29</v>
       </c>
-      <c r="G9" t="s">
+      <c r="H9" t="s">
         <v>30</v>
       </c>
-      <c r="H9" t="s">
+      <c r="I9" t="s">
         <v>31</v>
       </c>
-      <c r="I9" t="s">
+      <c r="J9" t="s">
         <v>32</v>
       </c>
-      <c r="J9" t="s">
+      <c r="K9" t="s">
         <v>33</v>
       </c>
-      <c r="K9" t="s">
+      <c r="L9" t="s">
         <v>34</v>
       </c>
-      <c r="L9" t="s">
+      <c r="M9" t="s">
         <v>35</v>
       </c>
-      <c r="M9" t="s">
+      <c r="N9" t="s">
         <v>36</v>
       </c>
-      <c r="N9" t="s">
+      <c r="O9" t="s">
         <v>37</v>
       </c>
-      <c r="O9" t="s">
+      <c r="P9" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q9" t="s">
         <v>38</v>
       </c>
-      <c r="P9" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q9" t="s">
+      <c r="R9" t="s">
         <v>39</v>
       </c>
-      <c r="R9" t="s">
+      <c r="S9" t="s">
         <v>40</v>
-      </c>
-      <c r="S9" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
@@ -1142,58 +1154,58 @@
         <v>9</v>
       </c>
       <c r="B10" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="C10" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="D10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E10" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F10" t="s">
+        <v>28</v>
+      </c>
+      <c r="G10" t="s">
         <v>29</v>
       </c>
-      <c r="G10" t="s">
+      <c r="H10" t="s">
         <v>30</v>
       </c>
-      <c r="H10" t="s">
+      <c r="I10" t="s">
         <v>31</v>
       </c>
-      <c r="I10" t="s">
+      <c r="J10" t="s">
         <v>32</v>
       </c>
-      <c r="J10" t="s">
+      <c r="K10" t="s">
         <v>33</v>
       </c>
-      <c r="K10" t="s">
+      <c r="L10" t="s">
         <v>34</v>
       </c>
-      <c r="L10" t="s">
+      <c r="M10" t="s">
         <v>35</v>
       </c>
-      <c r="M10" t="s">
+      <c r="N10" t="s">
         <v>36</v>
       </c>
-      <c r="N10" t="s">
+      <c r="O10" t="s">
         <v>37</v>
       </c>
-      <c r="O10" t="s">
+      <c r="P10" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q10" t="s">
         <v>38</v>
       </c>
-      <c r="P10" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q10" t="s">
+      <c r="R10" t="s">
         <v>39</v>
       </c>
-      <c r="R10" t="s">
+      <c r="S10" t="s">
         <v>40</v>
-      </c>
-      <c r="S10" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
@@ -1201,58 +1213,58 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E11" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F11" t="s">
+        <v>28</v>
+      </c>
+      <c r="G11" t="s">
         <v>29</v>
       </c>
-      <c r="G11" t="s">
+      <c r="H11" t="s">
         <v>30</v>
       </c>
-      <c r="H11" t="s">
+      <c r="I11" t="s">
         <v>31</v>
       </c>
-      <c r="I11" t="s">
+      <c r="J11" t="s">
         <v>32</v>
       </c>
-      <c r="J11" t="s">
+      <c r="K11" t="s">
         <v>33</v>
       </c>
-      <c r="K11" t="s">
+      <c r="L11" t="s">
         <v>34</v>
       </c>
-      <c r="L11" t="s">
+      <c r="M11" t="s">
         <v>35</v>
       </c>
-      <c r="M11" t="s">
+      <c r="N11" t="s">
         <v>36</v>
       </c>
-      <c r="N11" t="s">
+      <c r="O11" t="s">
         <v>37</v>
       </c>
-      <c r="O11" t="s">
+      <c r="P11" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q11" t="s">
         <v>38</v>
       </c>
-      <c r="P11" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q11" t="s">
+      <c r="R11" t="s">
         <v>39</v>
       </c>
-      <c r="R11" t="s">
+      <c r="S11" t="s">
         <v>40</v>
-      </c>
-      <c r="S11" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
@@ -1260,58 +1272,58 @@
         <v>11</v>
       </c>
       <c r="B12" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C12" t="s">
         <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E12" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F12" t="s">
+        <v>28</v>
+      </c>
+      <c r="G12" t="s">
         <v>29</v>
       </c>
-      <c r="G12" t="s">
+      <c r="H12" t="s">
         <v>30</v>
       </c>
-      <c r="H12" t="s">
+      <c r="I12" t="s">
         <v>31</v>
       </c>
-      <c r="I12" t="s">
+      <c r="J12" t="s">
         <v>32</v>
       </c>
-      <c r="J12" t="s">
+      <c r="K12" t="s">
         <v>33</v>
       </c>
-      <c r="K12" t="s">
+      <c r="L12" t="s">
         <v>34</v>
       </c>
-      <c r="L12" t="s">
+      <c r="M12" t="s">
         <v>35</v>
       </c>
-      <c r="M12" t="s">
+      <c r="N12" t="s">
         <v>36</v>
       </c>
-      <c r="N12" t="s">
+      <c r="O12" t="s">
         <v>37</v>
       </c>
-      <c r="O12" t="s">
+      <c r="P12" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q12" t="s">
         <v>38</v>
       </c>
-      <c r="P12" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q12" t="s">
+      <c r="R12" t="s">
         <v>39</v>
       </c>
-      <c r="R12" t="s">
+      <c r="S12" t="s">
         <v>40</v>
-      </c>
-      <c r="S12" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
@@ -1319,58 +1331,58 @@
         <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C13" t="s">
         <v>0</v>
       </c>
       <c r="D13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E13" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F13" t="s">
+        <v>28</v>
+      </c>
+      <c r="G13" t="s">
         <v>29</v>
       </c>
-      <c r="G13" t="s">
+      <c r="H13" t="s">
         <v>30</v>
       </c>
-      <c r="H13" t="s">
+      <c r="I13" t="s">
         <v>31</v>
       </c>
-      <c r="I13" t="s">
+      <c r="J13" t="s">
         <v>32</v>
       </c>
-      <c r="J13" t="s">
+      <c r="K13" t="s">
         <v>33</v>
       </c>
-      <c r="K13" t="s">
+      <c r="L13" t="s">
         <v>34</v>
       </c>
-      <c r="L13" t="s">
+      <c r="M13" t="s">
         <v>35</v>
       </c>
-      <c r="M13" t="s">
+      <c r="N13" t="s">
         <v>36</v>
       </c>
-      <c r="N13" t="s">
+      <c r="O13" t="s">
         <v>37</v>
       </c>
-      <c r="O13" t="s">
+      <c r="P13" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q13" t="s">
         <v>38</v>
       </c>
-      <c r="P13" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q13" t="s">
+      <c r="R13" t="s">
         <v>39</v>
       </c>
-      <c r="R13" t="s">
+      <c r="S13" t="s">
         <v>40</v>
-      </c>
-      <c r="S13" t="s">
-        <v>41</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
@@ -1378,55 +1390,55 @@
         <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="D14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="E14" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="F14" t="s">
+        <v>28</v>
+      </c>
+      <c r="G14" t="s">
         <v>29</v>
       </c>
-      <c r="G14" t="s">
+      <c r="H14" t="s">
         <v>30</v>
       </c>
-      <c r="H14" t="s">
+      <c r="I14" t="s">
         <v>31</v>
       </c>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
         <v>32</v>
       </c>
-      <c r="J14" t="s">
+      <c r="K14" t="s">
         <v>33</v>
       </c>
-      <c r="K14" t="s">
+      <c r="L14" t="s">
         <v>34</v>
       </c>
-      <c r="L14" t="s">
+      <c r="M14" t="s">
         <v>35</v>
       </c>
-      <c r="M14" t="s">
+      <c r="N14" t="s">
         <v>36</v>
       </c>
-      <c r="N14" t="s">
+      <c r="O14" t="s">
         <v>37</v>
       </c>
-      <c r="O14" t="s">
+      <c r="P14" t="s">
+        <v>41</v>
+      </c>
+      <c r="Q14" t="s">
         <v>38</v>
       </c>
-      <c r="P14" t="s">
-        <v>42</v>
-      </c>
-      <c r="Q14" t="s">
+      <c r="R14" t="s">
         <v>39</v>
       </c>
-      <c r="R14" t="s">
+      <c r="S14" t="s">
         <v>40</v>
-      </c>
-      <c r="S14" t="s">
-        <v>41</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added a new job
</commit_message>
<xml_diff>
--- a/Jobs/HomeJobs.xlsx
+++ b/Jobs/HomeJobs.xlsx
@@ -16,7 +16,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="142">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="191" uniqueCount="161">
   <si>
     <t>S.No</t>
   </si>
@@ -442,6 +442,63 @@
   </si>
   <si>
     <t>Canteen -free</t>
+  </si>
+  <si>
+    <t>Samkwang Mobile</t>
+  </si>
+  <si>
+    <t>kasna Gr Noida</t>
+  </si>
+  <si>
+    <t>SSR contractor में Boysकी भर्ती है आवशयकता है samkwang company के लिए</t>
+  </si>
+  <si>
+    <t>वर्क लोकेशन (फैक्ट्री) -: Samkwang india electronics pvt Ltd.. Company</t>
+  </si>
+  <si>
+    <t>Kasna , Greater Noida.</t>
+  </si>
+  <si>
+    <t>Department: Assembly</t>
+  </si>
+  <si>
+    <t>Salary = 10994  and  OT= 106 per hrs</t>
+  </si>
+  <si>
+    <t>योग्यता: 10th, 12 th,ITI</t>
+  </si>
+  <si>
+    <t>आवश्यक दस्तावेज़: resume 2 photo , photo copy all documents</t>
+  </si>
+  <si>
+    <t>अतिरिक्त लाभ: Double Overtime, Attend.Award- 700, Lunch/Canteen Free, Bus Free</t>
+  </si>
+  <si>
+    <t>Only for Boys</t>
+  </si>
+  <si>
+    <t>नोट- डॉक्यूमेंट के साथ आधार कार्ड और बैंक अकाउंट लाना अनिवार्य है (बैंक की पासबुक या चेक बुक)</t>
+  </si>
+  <si>
+    <t>न्यूनतम दूरी- 100 km</t>
+  </si>
+  <si>
+    <t>इंटरव्यू डेट :- *09/04/2025</t>
+  </si>
+  <si>
+    <t>Morning- 7:00 बजे</t>
+  </si>
+  <si>
+    <t>SS Research Solution Services</t>
+  </si>
+  <si>
+    <t>Contact: Abhishek Rawal-9990294311, Vivek-9368772854, Kush-7253035420, 9758570409 Ashish</t>
+  </si>
+  <si>
+    <t>Address: Plot No.1, Samkwang India Electronic Private limited, 10, Ecotech III, Greater Noida, Uttar Pradesh 203202</t>
+  </si>
+  <si>
+    <t>Google map: https://maps.app.goo.gl/kBG75cpD1WuKs6Tg9</t>
   </si>
 </sst>
 </file>
@@ -794,10 +851,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:X9"/>
+  <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="P14" sqref="P14"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="W2" sqref="W2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -882,14 +939,11 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
-      <c r="A2">
-        <v>1</v>
-      </c>
       <c r="B2" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="C2" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="D2" t="s">
         <v>33</v>
@@ -898,57 +952,66 @@
         <v>33</v>
       </c>
       <c r="F2" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="G2" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="H2" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="I2" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="J2" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="K2" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="L2" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="M2" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="N2" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="O2" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="P2" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="Q2" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="R2" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="S2" t="s">
-        <v>141</v>
+        <v>157</v>
+      </c>
+      <c r="T2" t="s">
+        <v>158</v>
+      </c>
+      <c r="U2" t="s">
+        <v>159</v>
+      </c>
+      <c r="V2" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="C3" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="D3" t="s">
         <v>33</v>
@@ -957,63 +1020,57 @@
         <v>33</v>
       </c>
       <c r="F3" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="G3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="H3" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="I3" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="J3" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="K3" t="s">
-        <v>31</v>
+        <v>133</v>
       </c>
       <c r="L3" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="M3" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="N3" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="O3" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="P3" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="Q3" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="R3" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="S3" t="s">
-        <v>120</v>
-      </c>
-      <c r="T3" t="s">
-        <v>121</v>
-      </c>
-      <c r="U3" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="C4" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="D4" t="s">
         <v>33</v>
@@ -1022,69 +1079,63 @@
         <v>33</v>
       </c>
       <c r="F4" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="G4" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="H4" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="I4" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="J4" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="K4" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="L4" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="M4" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="N4" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="O4" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="P4" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="Q4" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="R4" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="S4" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="T4" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="U4" t="s">
-        <v>106</v>
-      </c>
-      <c r="V4" t="s">
-        <v>107</v>
-      </c>
-      <c r="W4" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C5" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="D5" t="s">
         <v>33</v>
@@ -1093,42 +1144,69 @@
         <v>33</v>
       </c>
       <c r="F5" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="G5" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="H5" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="I5" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="J5" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="K5" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="L5" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="M5" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="N5" t="s">
-        <v>50</v>
+        <v>99</v>
+      </c>
+      <c r="O5" t="s">
+        <v>100</v>
+      </c>
+      <c r="P5" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>102</v>
+      </c>
+      <c r="R5" t="s">
+        <v>103</v>
+      </c>
+      <c r="S5" t="s">
+        <v>104</v>
+      </c>
+      <c r="T5" t="s">
+        <v>105</v>
+      </c>
+      <c r="U5" t="s">
+        <v>106</v>
+      </c>
+      <c r="V5" t="s">
+        <v>107</v>
+      </c>
+      <c r="W5" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C6" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="D6" t="s">
         <v>33</v>
@@ -1137,69 +1215,42 @@
         <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="G6" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="H6" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="I6" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="J6" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="K6" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="L6" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="M6" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="N6" t="s">
-        <v>80</v>
-      </c>
-      <c r="O6" t="s">
-        <v>81</v>
-      </c>
-      <c r="P6" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>83</v>
-      </c>
-      <c r="R6" t="s">
-        <v>84</v>
-      </c>
-      <c r="S6" t="s">
-        <v>85</v>
-      </c>
-      <c r="T6" t="s">
-        <v>86</v>
-      </c>
-      <c r="U6" t="s">
-        <v>87</v>
-      </c>
-      <c r="V6" t="s">
-        <v>88</v>
-      </c>
-      <c r="W6" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="C7" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="D7" t="s">
         <v>33</v>
@@ -1208,54 +1259,69 @@
         <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="G7" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="H7" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="I7" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="J7" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="K7" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="L7" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="M7" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="N7" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="O7" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="P7" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="Q7" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="R7" t="s">
-        <v>39</v>
+        <v>84</v>
+      </c>
+      <c r="S7" t="s">
+        <v>85</v>
+      </c>
+      <c r="T7" t="s">
+        <v>86</v>
+      </c>
+      <c r="U7" t="s">
+        <v>87</v>
+      </c>
+      <c r="V7" t="s">
+        <v>88</v>
+      </c>
+      <c r="W7" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C8" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D8" t="s">
         <v>33</v>
@@ -1264,98 +1330,154 @@
         <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="G8" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="H8" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="I8" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="J8" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="K8" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="L8" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="M8" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="N8" t="s">
-        <v>50</v>
+        <v>36</v>
+      </c>
+      <c r="O8" t="s">
+        <v>38</v>
+      </c>
+      <c r="P8" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q8" t="s">
+        <v>31</v>
+      </c>
+      <c r="R8" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
+        <v>40</v>
+      </c>
+      <c r="C9" t="s">
+        <v>41</v>
+      </c>
+      <c r="D9" t="s">
+        <v>33</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
+      </c>
+      <c r="F9" t="s">
+        <v>42</v>
+      </c>
+      <c r="G9" t="s">
+        <v>44</v>
+      </c>
+      <c r="H9" t="s">
+        <v>43</v>
+      </c>
+      <c r="I9" t="s">
+        <v>45</v>
+      </c>
+      <c r="J9" t="s">
+        <v>46</v>
+      </c>
+      <c r="K9" t="s">
+        <v>47</v>
+      </c>
+      <c r="L9" t="s">
+        <v>48</v>
+      </c>
+      <c r="M9" t="s">
+        <v>49</v>
+      </c>
+      <c r="N9" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="10" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A10">
         <v>8</v>
       </c>
-      <c r="B9" t="s">
+      <c r="B10" t="s">
         <v>51</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C10" t="s">
         <v>52</v>
       </c>
-      <c r="D9" t="s">
-        <v>33</v>
-      </c>
-      <c r="E9" t="s">
-        <v>33</v>
-      </c>
-      <c r="F9" t="s">
+      <c r="D10" t="s">
+        <v>33</v>
+      </c>
+      <c r="E10" t="s">
+        <v>33</v>
+      </c>
+      <c r="F10" t="s">
         <v>55</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G10" t="s">
         <v>54</v>
       </c>
-      <c r="H9" t="s">
+      <c r="H10" t="s">
         <v>53</v>
       </c>
-      <c r="I9" t="s">
+      <c r="I10" t="s">
         <v>56</v>
       </c>
-      <c r="J9" t="s">
+      <c r="J10" t="s">
         <v>57</v>
       </c>
-      <c r="K9" t="s">
+      <c r="K10" t="s">
         <v>58</v>
       </c>
-      <c r="L9" t="s">
+      <c r="L10" t="s">
         <v>59</v>
       </c>
-      <c r="M9" t="s">
+      <c r="M10" t="s">
         <v>60</v>
       </c>
-      <c r="N9" t="s">
+      <c r="N10" t="s">
         <v>61</v>
       </c>
-      <c r="O9" t="s">
+      <c r="O10" t="s">
         <v>62</v>
       </c>
-      <c r="P9" t="s">
+      <c r="P10" t="s">
         <v>63</v>
       </c>
-      <c r="Q9" t="s">
+      <c r="Q10" t="s">
         <v>64</v>
       </c>
-      <c r="R9" t="s">
+      <c r="R10" t="s">
         <v>65</v>
       </c>
-      <c r="S9" t="s">
+      <c r="S10" t="s">
         <v>66</v>
       </c>
-      <c r="T9" t="s">
+      <c r="T10" t="s">
         <v>67</v>
       </c>
-      <c r="U9" t="s">
+      <c r="U10" t="s">
         <v>68</v>
       </c>
-      <c r="V9" t="s">
+      <c r="V10" t="s">
         <v>69</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Corrected the job ID
</commit_message>
<xml_diff>
--- a/Jobs/HomeJobs.xlsx
+++ b/Jobs/HomeJobs.xlsx
@@ -853,8 +853,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X10"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="W2" sqref="W2"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:A10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -939,6 +939,9 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>1</v>
+      </c>
       <c r="B2" t="s">
         <v>142</v>
       </c>
@@ -1005,7 +1008,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
         <v>126</v>
@@ -1064,7 +1067,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -1129,7 +1132,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B5" t="s">
         <v>90</v>
@@ -1200,7 +1203,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
@@ -1244,7 +1247,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
@@ -1315,7 +1318,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -1371,7 +1374,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
         <v>40</v>
@@ -1415,7 +1418,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B10" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
Changed the job id
</commit_message>
<xml_diff>
--- a/Jobs/HomeJobs.xlsx
+++ b/Jobs/HomeJobs.xlsx
@@ -854,7 +854,7 @@
   <dimension ref="A1:X10"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2:A10"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -940,7 +940,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B2" t="s">
         <v>142</v>
@@ -1008,7 +1008,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
         <v>126</v>
@@ -1067,7 +1067,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
         <v>24</v>
@@ -1132,7 +1132,7 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
         <v>90</v>
@@ -1203,7 +1203,7 @@
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
         <v>40</v>
@@ -1247,7 +1247,7 @@
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
         <v>70</v>
@@ -1318,7 +1318,7 @@
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
         <v>24</v>
@@ -1374,7 +1374,7 @@
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
         <v>40</v>
@@ -1418,7 +1418,7 @@
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
         <v>51</v>

</xml_diff>

<commit_message>
added the job ID
</commit_message>
<xml_diff>
--- a/Jobs/HomeJobs.xlsx
+++ b/Jobs/HomeJobs.xlsx
@@ -1019,7 +1019,7 @@
   <dimension ref="A1:X14"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="T2" sqref="T2"/>
+      <selection activeCell="B11" sqref="B11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1104,6 +1104,9 @@
       </c>
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
+      <c r="A2">
+        <v>13</v>
+      </c>
       <c r="B2" t="s">
         <v>200</v>
       </c>

</xml_diff>

<commit_message>
Removed the commented code and corrected the job ID
</commit_message>
<xml_diff>
--- a/Jobs/HomeJobs.xlsx
+++ b/Jobs/HomeJobs.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9302"/>
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="5" rupBuild="9303"/>
   <workbookPr defaultThemeVersion="124226"/>
   <bookViews>
     <workbookView xWindow="240" yWindow="60" windowWidth="20115" windowHeight="8010"/>
@@ -1543,8 +1543,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:X28"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A10" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1646,7 +1646,7 @@
     </row>
     <row r="2" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A2">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
         <v>379</v>
@@ -1696,7 +1696,7 @@
     </row>
     <row r="3" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A3">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
         <v>372</v>
@@ -1731,7 +1731,7 @@
     </row>
     <row r="4" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A4">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B4" t="s">
         <v>355</v>
@@ -1775,10 +1775,10 @@
     </row>
     <row r="5" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A5">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B5" t="s">
-        <v>344</v>
+        <v>365</v>
       </c>
       <c r="C5" t="s">
         <v>345</v>
@@ -1789,43 +1789,37 @@
       <c r="E5" t="s">
         <v>33</v>
       </c>
-      <c r="F5" t="s">
-        <v>346</v>
+      <c r="F5" s="4" t="s">
+        <v>366</v>
       </c>
       <c r="G5" t="s">
-        <v>347</v>
+        <v>367</v>
       </c>
       <c r="H5" t="s">
-        <v>348</v>
+        <v>368</v>
       </c>
       <c r="I5" t="s">
-        <v>349</v>
+        <v>371</v>
       </c>
       <c r="J5" t="s">
-        <v>350</v>
+        <v>369</v>
       </c>
       <c r="K5" t="s">
-        <v>351</v>
+        <v>370</v>
       </c>
       <c r="L5" t="s">
-        <v>352</v>
-      </c>
-      <c r="M5" t="s">
-        <v>353</v>
-      </c>
-      <c r="N5" t="s">
-        <v>354</v>
+        <v>360</v>
       </c>
     </row>
     <row r="6" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A6">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B6" t="s">
-        <v>327</v>
+        <v>344</v>
       </c>
       <c r="C6" t="s">
-        <v>328</v>
+        <v>345</v>
       </c>
       <c r="D6" t="s">
         <v>33</v>
@@ -1834,60 +1828,42 @@
         <v>33</v>
       </c>
       <c r="F6" t="s">
-        <v>329</v>
+        <v>346</v>
       </c>
       <c r="G6" t="s">
-        <v>330</v>
+        <v>347</v>
       </c>
       <c r="H6" t="s">
-        <v>331</v>
+        <v>348</v>
       </c>
       <c r="I6" t="s">
-        <v>332</v>
+        <v>349</v>
       </c>
       <c r="J6" t="s">
-        <v>333</v>
+        <v>350</v>
       </c>
       <c r="K6" t="s">
-        <v>334</v>
+        <v>351</v>
       </c>
       <c r="L6" t="s">
-        <v>335</v>
+        <v>352</v>
       </c>
       <c r="M6" t="s">
-        <v>336</v>
+        <v>353</v>
       </c>
       <c r="N6" t="s">
-        <v>337</v>
-      </c>
-      <c r="O6" t="s">
-        <v>338</v>
-      </c>
-      <c r="P6" t="s">
-        <v>339</v>
-      </c>
-      <c r="Q6" t="s">
-        <v>340</v>
-      </c>
-      <c r="R6" t="s">
-        <v>341</v>
-      </c>
-      <c r="S6" t="s">
-        <v>342</v>
-      </c>
-      <c r="T6" t="s">
-        <v>343</v>
+        <v>354</v>
       </c>
     </row>
     <row r="7" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A7">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>310</v>
+        <v>327</v>
       </c>
       <c r="C7" t="s">
-        <v>71</v>
+        <v>328</v>
       </c>
       <c r="D7" t="s">
         <v>33</v>
@@ -1896,69 +1872,60 @@
         <v>33</v>
       </c>
       <c r="F7" t="s">
-        <v>311</v>
+        <v>329</v>
       </c>
       <c r="G7" t="s">
-        <v>312</v>
+        <v>330</v>
       </c>
       <c r="H7" t="s">
-        <v>314</v>
+        <v>331</v>
       </c>
       <c r="I7" t="s">
-        <v>313</v>
+        <v>332</v>
       </c>
       <c r="J7" t="s">
-        <v>315</v>
+        <v>333</v>
       </c>
       <c r="K7" t="s">
-        <v>316</v>
+        <v>334</v>
       </c>
       <c r="L7" t="s">
-        <v>317</v>
+        <v>335</v>
       </c>
       <c r="M7" t="s">
-        <v>318</v>
+        <v>336</v>
       </c>
       <c r="N7" t="s">
-        <v>319</v>
+        <v>337</v>
       </c>
       <c r="O7" t="s">
-        <v>250</v>
+        <v>338</v>
       </c>
       <c r="P7" t="s">
-        <v>320</v>
+        <v>339</v>
       </c>
       <c r="Q7" t="s">
-        <v>321</v>
+        <v>340</v>
       </c>
       <c r="R7" t="s">
-        <v>322</v>
+        <v>341</v>
       </c>
       <c r="S7" t="s">
-        <v>269</v>
+        <v>342</v>
       </c>
       <c r="T7" t="s">
-        <v>323</v>
-      </c>
-      <c r="U7" t="s">
-        <v>324</v>
-      </c>
-      <c r="V7" t="s">
-        <v>325</v>
-      </c>
-      <c r="W7" t="s">
-        <v>326</v>
+        <v>343</v>
       </c>
     </row>
     <row r="8" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A8">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B8" t="s">
-        <v>126</v>
+        <v>310</v>
       </c>
       <c r="C8" t="s">
-        <v>295</v>
+        <v>71</v>
       </c>
       <c r="D8" t="s">
         <v>33</v>
@@ -1967,66 +1934,69 @@
         <v>33</v>
       </c>
       <c r="F8" t="s">
-        <v>296</v>
+        <v>311</v>
       </c>
       <c r="G8" t="s">
-        <v>297</v>
+        <v>312</v>
       </c>
       <c r="H8" t="s">
-        <v>298</v>
+        <v>314</v>
       </c>
       <c r="I8" t="s">
-        <v>299</v>
+        <v>313</v>
       </c>
       <c r="J8" t="s">
-        <v>300</v>
+        <v>315</v>
       </c>
       <c r="K8" t="s">
-        <v>301</v>
+        <v>316</v>
       </c>
       <c r="L8" t="s">
-        <v>302</v>
+        <v>317</v>
       </c>
       <c r="M8" t="s">
-        <v>296</v>
+        <v>318</v>
       </c>
       <c r="N8" t="s">
-        <v>303</v>
+        <v>319</v>
       </c>
       <c r="O8" t="s">
-        <v>304</v>
+        <v>250</v>
       </c>
       <c r="P8" t="s">
-        <v>138</v>
+        <v>320</v>
       </c>
       <c r="Q8" t="s">
-        <v>305</v>
+        <v>321</v>
       </c>
       <c r="R8" t="s">
-        <v>306</v>
+        <v>322</v>
       </c>
       <c r="S8" t="s">
-        <v>307</v>
+        <v>269</v>
       </c>
       <c r="T8" t="s">
-        <v>308</v>
+        <v>323</v>
       </c>
       <c r="U8" t="s">
-        <v>131</v>
+        <v>324</v>
       </c>
       <c r="V8" t="s">
-        <v>309</v>
+        <v>325</v>
+      </c>
+      <c r="W8" t="s">
+        <v>326</v>
       </c>
     </row>
     <row r="9" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A9">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>142</v>
+        <v>126</v>
       </c>
       <c r="C9" t="s">
-        <v>71</v>
+        <v>295</v>
       </c>
       <c r="D9" t="s">
         <v>33</v>
@@ -2035,60 +2005,63 @@
         <v>33</v>
       </c>
       <c r="F9" t="s">
-        <v>144</v>
+        <v>296</v>
       </c>
       <c r="G9" t="s">
-        <v>145</v>
+        <v>297</v>
       </c>
       <c r="H9" t="s">
-        <v>285</v>
+        <v>298</v>
       </c>
       <c r="I9" t="s">
-        <v>286</v>
+        <v>299</v>
       </c>
       <c r="J9" t="s">
-        <v>156</v>
+        <v>300</v>
       </c>
       <c r="K9" t="s">
-        <v>287</v>
+        <v>301</v>
       </c>
       <c r="L9" t="s">
-        <v>288</v>
+        <v>302</v>
       </c>
       <c r="M9" t="s">
-        <v>289</v>
+        <v>296</v>
       </c>
       <c r="N9" t="s">
-        <v>290</v>
+        <v>303</v>
       </c>
       <c r="O9" t="s">
-        <v>181</v>
+        <v>304</v>
       </c>
       <c r="P9" t="s">
-        <v>291</v>
+        <v>138</v>
       </c>
       <c r="Q9" t="s">
-        <v>292</v>
+        <v>305</v>
       </c>
       <c r="R9" t="s">
-        <v>293</v>
+        <v>306</v>
       </c>
       <c r="S9" t="s">
-        <v>153</v>
+        <v>307</v>
       </c>
       <c r="T9" t="s">
-        <v>294</v>
+        <v>308</v>
       </c>
       <c r="U9" t="s">
-        <v>159</v>
+        <v>131</v>
+      </c>
+      <c r="V9" t="s">
+        <v>309</v>
       </c>
     </row>
     <row r="10" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A10">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B10" t="s">
-        <v>272</v>
+        <v>142</v>
       </c>
       <c r="C10" t="s">
         <v>71</v>
@@ -2100,48 +2073,63 @@
         <v>33</v>
       </c>
       <c r="F10" t="s">
-        <v>273</v>
+        <v>144</v>
       </c>
       <c r="G10" t="s">
-        <v>275</v>
+        <v>145</v>
       </c>
       <c r="H10" t="s">
-        <v>276</v>
+        <v>285</v>
       </c>
       <c r="I10" t="s">
-        <v>277</v>
+        <v>286</v>
       </c>
       <c r="J10" t="s">
-        <v>278</v>
+        <v>156</v>
       </c>
       <c r="K10" t="s">
-        <v>279</v>
+        <v>287</v>
       </c>
       <c r="L10" t="s">
-        <v>280</v>
+        <v>288</v>
       </c>
       <c r="M10" t="s">
-        <v>281</v>
+        <v>289</v>
       </c>
       <c r="N10" t="s">
-        <v>282</v>
+        <v>290</v>
       </c>
       <c r="O10" t="s">
-        <v>283</v>
+        <v>181</v>
       </c>
       <c r="P10" t="s">
-        <v>284</v>
+        <v>291</v>
+      </c>
+      <c r="Q10" t="s">
+        <v>292</v>
+      </c>
+      <c r="R10" t="s">
+        <v>293</v>
+      </c>
+      <c r="S10" t="s">
+        <v>153</v>
+      </c>
+      <c r="T10" t="s">
+        <v>294</v>
+      </c>
+      <c r="U10" t="s">
+        <v>159</v>
       </c>
     </row>
     <row r="11" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A11">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="B11" t="s">
-        <v>261</v>
+        <v>272</v>
       </c>
       <c r="C11" t="s">
-        <v>262</v>
+        <v>71</v>
       </c>
       <c r="D11" t="s">
         <v>33</v>
@@ -2150,48 +2138,48 @@
         <v>33</v>
       </c>
       <c r="F11" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="G11" t="s">
-        <v>263</v>
+        <v>275</v>
       </c>
       <c r="H11" t="s">
-        <v>264</v>
+        <v>276</v>
       </c>
       <c r="I11" t="s">
-        <v>265</v>
+        <v>277</v>
       </c>
       <c r="J11" t="s">
-        <v>266</v>
+        <v>278</v>
       </c>
       <c r="K11" t="s">
-        <v>250</v>
+        <v>279</v>
       </c>
       <c r="L11" t="s">
-        <v>267</v>
+        <v>280</v>
       </c>
       <c r="M11" t="s">
-        <v>268</v>
+        <v>281</v>
       </c>
       <c r="N11" t="s">
-        <v>269</v>
+        <v>282</v>
       </c>
       <c r="O11" t="s">
-        <v>270</v>
+        <v>283</v>
       </c>
       <c r="P11" t="s">
-        <v>271</v>
+        <v>284</v>
       </c>
     </row>
     <row r="12" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A12">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B12" t="s">
-        <v>244</v>
+        <v>261</v>
       </c>
       <c r="C12" t="s">
-        <v>71</v>
+        <v>262</v>
       </c>
       <c r="D12" t="s">
         <v>33</v>
@@ -2200,63 +2188,48 @@
         <v>33</v>
       </c>
       <c r="F12" t="s">
-        <v>245</v>
+        <v>274</v>
       </c>
       <c r="G12" t="s">
-        <v>246</v>
+        <v>263</v>
       </c>
       <c r="H12" t="s">
-        <v>257</v>
+        <v>264</v>
       </c>
       <c r="I12" t="s">
-        <v>248</v>
+        <v>265</v>
       </c>
       <c r="J12" t="s">
-        <v>247</v>
+        <v>266</v>
       </c>
       <c r="K12" t="s">
-        <v>249</v>
+        <v>250</v>
       </c>
       <c r="L12" t="s">
-        <v>250</v>
+        <v>267</v>
       </c>
       <c r="M12" t="s">
-        <v>251</v>
+        <v>268</v>
       </c>
       <c r="N12" t="s">
-        <v>252</v>
+        <v>269</v>
       </c>
       <c r="O12" t="s">
-        <v>253</v>
+        <v>270</v>
       </c>
       <c r="P12" t="s">
-        <v>254</v>
-      </c>
-      <c r="Q12" t="s">
-        <v>255</v>
-      </c>
-      <c r="R12" t="s">
-        <v>256</v>
-      </c>
-      <c r="S12" t="s">
-        <v>258</v>
-      </c>
-      <c r="T12" t="s">
-        <v>259</v>
-      </c>
-      <c r="U12" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
     </row>
     <row r="13" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A13">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B13" t="s">
-        <v>231</v>
+        <v>244</v>
       </c>
       <c r="C13" t="s">
-        <v>232</v>
+        <v>71</v>
       </c>
       <c r="D13" t="s">
         <v>33</v>
@@ -2265,48 +2238,63 @@
         <v>33</v>
       </c>
       <c r="F13" t="s">
-        <v>234</v>
+        <v>245</v>
       </c>
       <c r="G13" t="s">
-        <v>235</v>
+        <v>246</v>
       </c>
       <c r="H13" t="s">
-        <v>236</v>
+        <v>257</v>
       </c>
       <c r="I13" t="s">
-        <v>233</v>
+        <v>248</v>
       </c>
       <c r="J13" t="s">
-        <v>237</v>
+        <v>247</v>
       </c>
       <c r="K13" t="s">
-        <v>238</v>
+        <v>249</v>
       </c>
       <c r="L13" t="s">
-        <v>239</v>
+        <v>250</v>
       </c>
       <c r="M13" t="s">
-        <v>240</v>
+        <v>251</v>
       </c>
       <c r="N13" t="s">
-        <v>241</v>
+        <v>252</v>
       </c>
       <c r="O13" t="s">
-        <v>242</v>
+        <v>253</v>
       </c>
       <c r="P13" t="s">
-        <v>243</v>
+        <v>254</v>
+      </c>
+      <c r="Q13" t="s">
+        <v>255</v>
+      </c>
+      <c r="R13" t="s">
+        <v>256</v>
+      </c>
+      <c r="S13" t="s">
+        <v>258</v>
+      </c>
+      <c r="T13" t="s">
+        <v>259</v>
+      </c>
+      <c r="U13" t="s">
+        <v>260</v>
       </c>
     </row>
     <row r="14" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A14">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B14" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="C14" t="s">
-        <v>217</v>
+        <v>232</v>
       </c>
       <c r="D14" t="s">
         <v>33</v>
@@ -2315,54 +2303,48 @@
         <v>33</v>
       </c>
       <c r="F14" t="s">
-        <v>218</v>
+        <v>234</v>
       </c>
       <c r="G14" t="s">
-        <v>219</v>
+        <v>235</v>
       </c>
       <c r="H14" t="s">
-        <v>220</v>
+        <v>236</v>
       </c>
       <c r="I14" t="s">
-        <v>221</v>
+        <v>233</v>
       </c>
       <c r="J14" t="s">
-        <v>222</v>
+        <v>237</v>
       </c>
       <c r="K14" t="s">
-        <v>223</v>
+        <v>238</v>
       </c>
       <c r="L14" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="M14" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="N14" t="s">
-        <v>226</v>
+        <v>241</v>
       </c>
       <c r="O14" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
       <c r="P14" t="s">
-        <v>228</v>
-      </c>
-      <c r="Q14" t="s">
-        <v>229</v>
-      </c>
-      <c r="R14" t="s">
-        <v>230</v>
+        <v>243</v>
       </c>
     </row>
     <row r="15" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A15">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>200</v>
+        <v>216</v>
       </c>
       <c r="C15" t="s">
-        <v>201</v>
+        <v>217</v>
       </c>
       <c r="D15" t="s">
         <v>33</v>
@@ -2371,57 +2353,54 @@
         <v>33</v>
       </c>
       <c r="F15" t="s">
-        <v>202</v>
+        <v>218</v>
       </c>
       <c r="G15" t="s">
-        <v>203</v>
+        <v>219</v>
       </c>
       <c r="H15" t="s">
-        <v>204</v>
+        <v>220</v>
       </c>
       <c r="I15" t="s">
-        <v>205</v>
+        <v>221</v>
       </c>
       <c r="J15" t="s">
-        <v>206</v>
+        <v>222</v>
       </c>
       <c r="K15" t="s">
-        <v>207</v>
+        <v>223</v>
       </c>
       <c r="L15" t="s">
-        <v>208</v>
+        <v>224</v>
       </c>
       <c r="M15" t="s">
-        <v>209</v>
+        <v>225</v>
       </c>
       <c r="N15" t="s">
-        <v>210</v>
+        <v>226</v>
       </c>
       <c r="O15" t="s">
-        <v>211</v>
+        <v>227</v>
       </c>
       <c r="P15" t="s">
-        <v>212</v>
+        <v>228</v>
       </c>
       <c r="Q15" t="s">
-        <v>213</v>
+        <v>229</v>
       </c>
       <c r="R15" t="s">
-        <v>214</v>
-      </c>
-      <c r="S15" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
     </row>
     <row r="16" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A16">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B16" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="C16" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="D16" t="s">
         <v>33</v>
@@ -2430,54 +2409,57 @@
         <v>33</v>
       </c>
       <c r="F16" t="s">
-        <v>187</v>
+        <v>202</v>
       </c>
       <c r="G16" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
       <c r="H16" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="I16" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="J16" t="s">
-        <v>191</v>
+        <v>206</v>
       </c>
       <c r="K16" t="s">
-        <v>192</v>
+        <v>207</v>
       </c>
       <c r="L16" t="s">
-        <v>193</v>
+        <v>208</v>
       </c>
       <c r="M16" t="s">
-        <v>195</v>
+        <v>209</v>
       </c>
       <c r="N16" t="s">
-        <v>194</v>
+        <v>210</v>
       </c>
       <c r="O16" t="s">
-        <v>196</v>
+        <v>211</v>
       </c>
       <c r="P16" t="s">
-        <v>197</v>
+        <v>212</v>
       </c>
       <c r="Q16" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="R16" t="s">
-        <v>199</v>
+        <v>214</v>
+      </c>
+      <c r="S16" t="s">
+        <v>215</v>
       </c>
     </row>
     <row r="17" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A17">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B17" t="s">
-        <v>172</v>
+        <v>185</v>
       </c>
       <c r="C17" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="D17" t="s">
         <v>33</v>
@@ -2486,57 +2468,54 @@
         <v>33</v>
       </c>
       <c r="F17" t="s">
-        <v>173</v>
+        <v>187</v>
       </c>
       <c r="G17" t="s">
-        <v>175</v>
+        <v>188</v>
       </c>
       <c r="H17" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
       <c r="I17" t="s">
-        <v>176</v>
+        <v>190</v>
       </c>
       <c r="J17" t="s">
-        <v>177</v>
+        <v>191</v>
       </c>
       <c r="K17" t="s">
-        <v>178</v>
+        <v>192</v>
       </c>
       <c r="L17" t="s">
-        <v>150</v>
+        <v>193</v>
       </c>
       <c r="M17" t="s">
-        <v>179</v>
+        <v>195</v>
       </c>
       <c r="N17" t="s">
-        <v>180</v>
+        <v>194</v>
       </c>
       <c r="O17" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="P17" t="s">
-        <v>153</v>
+        <v>197</v>
       </c>
       <c r="Q17" t="s">
-        <v>182</v>
+        <v>198</v>
       </c>
       <c r="R17" t="s">
-        <v>183</v>
-      </c>
-      <c r="S17" t="s">
-        <v>184</v>
+        <v>199</v>
       </c>
     </row>
     <row r="18" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A18">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B18" t="s">
-        <v>161</v>
+        <v>172</v>
       </c>
       <c r="C18" t="s">
-        <v>162</v>
+        <v>171</v>
       </c>
       <c r="D18" t="s">
         <v>33</v>
@@ -2545,72 +2524,57 @@
         <v>33</v>
       </c>
       <c r="F18" t="s">
-        <v>91</v>
+        <v>173</v>
       </c>
       <c r="G18" t="s">
-        <v>163</v>
+        <v>175</v>
       </c>
       <c r="H18" t="s">
-        <v>164</v>
+        <v>174</v>
       </c>
       <c r="I18" t="s">
-        <v>165</v>
+        <v>176</v>
       </c>
       <c r="J18" t="s">
-        <v>94</v>
+        <v>177</v>
       </c>
       <c r="K18" t="s">
-        <v>95</v>
+        <v>178</v>
       </c>
       <c r="L18" t="s">
-        <v>96</v>
+        <v>150</v>
       </c>
       <c r="M18" t="s">
-        <v>97</v>
+        <v>179</v>
       </c>
       <c r="N18" t="s">
-        <v>166</v>
+        <v>180</v>
       </c>
       <c r="O18" t="s">
-        <v>167</v>
+        <v>181</v>
       </c>
       <c r="P18" t="s">
-        <v>168</v>
+        <v>153</v>
       </c>
       <c r="Q18" t="s">
-        <v>102</v>
+        <v>182</v>
       </c>
       <c r="R18" t="s">
-        <v>103</v>
+        <v>183</v>
       </c>
       <c r="S18" t="s">
-        <v>169</v>
-      </c>
-      <c r="T18" t="s">
-        <v>170</v>
-      </c>
-      <c r="U18" t="s">
-        <v>105</v>
-      </c>
-      <c r="V18" t="s">
-        <v>106</v>
-      </c>
-      <c r="W18" t="s">
-        <v>107</v>
-      </c>
-      <c r="X18" t="s">
-        <v>108</v>
+        <v>184</v>
       </c>
     </row>
     <row r="19" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A19">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>142</v>
+        <v>161</v>
       </c>
       <c r="C19" t="s">
-        <v>143</v>
+        <v>162</v>
       </c>
       <c r="D19" t="s">
         <v>33</v>
@@ -2619,66 +2583,72 @@
         <v>33</v>
       </c>
       <c r="F19" t="s">
-        <v>144</v>
+        <v>91</v>
       </c>
       <c r="G19" t="s">
-        <v>145</v>
+        <v>163</v>
       </c>
       <c r="H19" t="s">
-        <v>146</v>
+        <v>164</v>
       </c>
       <c r="I19" t="s">
-        <v>147</v>
+        <v>165</v>
       </c>
       <c r="J19" t="s">
-        <v>148</v>
+        <v>94</v>
       </c>
       <c r="K19" t="s">
-        <v>149</v>
+        <v>95</v>
       </c>
       <c r="L19" t="s">
-        <v>150</v>
+        <v>96</v>
       </c>
       <c r="M19" t="s">
-        <v>151</v>
+        <v>97</v>
       </c>
       <c r="N19" t="s">
-        <v>152</v>
+        <v>166</v>
       </c>
       <c r="O19" t="s">
-        <v>153</v>
+        <v>167</v>
       </c>
       <c r="P19" t="s">
-        <v>154</v>
+        <v>168</v>
       </c>
       <c r="Q19" t="s">
-        <v>155</v>
+        <v>102</v>
       </c>
       <c r="R19" t="s">
-        <v>156</v>
+        <v>103</v>
       </c>
       <c r="S19" t="s">
-        <v>157</v>
+        <v>169</v>
       </c>
       <c r="T19" t="s">
-        <v>158</v>
+        <v>170</v>
       </c>
       <c r="U19" t="s">
-        <v>159</v>
+        <v>105</v>
       </c>
       <c r="V19" t="s">
-        <v>160</v>
+        <v>106</v>
+      </c>
+      <c r="W19" t="s">
+        <v>107</v>
+      </c>
+      <c r="X19" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="20" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A20">
-        <v>1</v>
+        <v>9</v>
       </c>
       <c r="B20" t="s">
-        <v>126</v>
+        <v>142</v>
       </c>
       <c r="C20" t="s">
-        <v>127</v>
+        <v>143</v>
       </c>
       <c r="D20" t="s">
         <v>33</v>
@@ -2687,57 +2657,66 @@
         <v>33</v>
       </c>
       <c r="F20" t="s">
-        <v>128</v>
+        <v>144</v>
       </c>
       <c r="G20" t="s">
-        <v>129</v>
+        <v>145</v>
       </c>
       <c r="H20" t="s">
-        <v>130</v>
+        <v>146</v>
       </c>
       <c r="I20" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="J20" t="s">
-        <v>131</v>
+        <v>148</v>
       </c>
       <c r="K20" t="s">
-        <v>133</v>
+        <v>149</v>
       </c>
       <c r="L20" t="s">
-        <v>134</v>
+        <v>150</v>
       </c>
       <c r="M20" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="N20" t="s">
-        <v>135</v>
+        <v>152</v>
       </c>
       <c r="O20" t="s">
-        <v>137</v>
+        <v>153</v>
       </c>
       <c r="P20" t="s">
-        <v>138</v>
+        <v>154</v>
       </c>
       <c r="Q20" t="s">
-        <v>139</v>
+        <v>155</v>
       </c>
       <c r="R20" t="s">
-        <v>140</v>
+        <v>156</v>
       </c>
       <c r="S20" t="s">
-        <v>141</v>
+        <v>157</v>
+      </c>
+      <c r="T20" t="s">
+        <v>158</v>
+      </c>
+      <c r="U20" t="s">
+        <v>159</v>
+      </c>
+      <c r="V20" t="s">
+        <v>160</v>
       </c>
     </row>
     <row r="21" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A21">
-        <v>2</v>
+        <v>1</v>
       </c>
       <c r="B21" t="s">
-        <v>24</v>
+        <v>126</v>
       </c>
       <c r="C21" t="s">
-        <v>111</v>
+        <v>127</v>
       </c>
       <c r="D21" t="s">
         <v>33</v>
@@ -2746,63 +2725,57 @@
         <v>33</v>
       </c>
       <c r="F21" t="s">
-        <v>110</v>
+        <v>128</v>
       </c>
       <c r="G21" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="H21" t="s">
-        <v>113</v>
+        <v>130</v>
       </c>
       <c r="I21" t="s">
-        <v>114</v>
+        <v>132</v>
       </c>
       <c r="J21" t="s">
-        <v>115</v>
+        <v>131</v>
       </c>
       <c r="K21" t="s">
-        <v>31</v>
+        <v>133</v>
       </c>
       <c r="L21" t="s">
-        <v>116</v>
+        <v>134</v>
       </c>
       <c r="M21" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="N21" t="s">
-        <v>118</v>
+        <v>135</v>
       </c>
       <c r="O21" t="s">
-        <v>119</v>
+        <v>137</v>
       </c>
       <c r="P21" t="s">
-        <v>124</v>
+        <v>138</v>
       </c>
       <c r="Q21" t="s">
-        <v>123</v>
+        <v>139</v>
       </c>
       <c r="R21" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="S21" t="s">
-        <v>120</v>
-      </c>
-      <c r="T21" t="s">
-        <v>121</v>
-      </c>
-      <c r="U21" t="s">
-        <v>122</v>
+        <v>141</v>
       </c>
     </row>
     <row r="22" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A22">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B22" t="s">
-        <v>90</v>
+        <v>24</v>
       </c>
       <c r="C22" t="s">
-        <v>71</v>
+        <v>111</v>
       </c>
       <c r="D22" t="s">
         <v>33</v>
@@ -2811,69 +2784,63 @@
         <v>33</v>
       </c>
       <c r="F22" t="s">
-        <v>91</v>
+        <v>110</v>
       </c>
       <c r="G22" t="s">
-        <v>92</v>
+        <v>112</v>
       </c>
       <c r="H22" t="s">
-        <v>93</v>
+        <v>113</v>
       </c>
       <c r="I22" t="s">
-        <v>94</v>
+        <v>114</v>
       </c>
       <c r="J22" t="s">
-        <v>95</v>
+        <v>115</v>
       </c>
       <c r="K22" t="s">
-        <v>96</v>
+        <v>31</v>
       </c>
       <c r="L22" t="s">
-        <v>97</v>
+        <v>116</v>
       </c>
       <c r="M22" t="s">
-        <v>98</v>
+        <v>117</v>
       </c>
       <c r="N22" t="s">
-        <v>99</v>
+        <v>118</v>
       </c>
       <c r="O22" t="s">
-        <v>100</v>
+        <v>119</v>
       </c>
       <c r="P22" t="s">
-        <v>101</v>
+        <v>124</v>
       </c>
       <c r="Q22" t="s">
-        <v>102</v>
+        <v>123</v>
       </c>
       <c r="R22" t="s">
-        <v>103</v>
+        <v>125</v>
       </c>
       <c r="S22" t="s">
-        <v>104</v>
+        <v>120</v>
       </c>
       <c r="T22" t="s">
-        <v>105</v>
+        <v>121</v>
       </c>
       <c r="U22" t="s">
-        <v>106</v>
-      </c>
-      <c r="V22" t="s">
-        <v>107</v>
-      </c>
-      <c r="W22" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
     </row>
     <row r="23" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A23">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B23" t="s">
-        <v>40</v>
+        <v>90</v>
       </c>
       <c r="C23" t="s">
-        <v>41</v>
+        <v>71</v>
       </c>
       <c r="D23" t="s">
         <v>33</v>
@@ -2882,42 +2849,69 @@
         <v>33</v>
       </c>
       <c r="F23" t="s">
-        <v>42</v>
+        <v>91</v>
       </c>
       <c r="G23" t="s">
-        <v>109</v>
+        <v>92</v>
       </c>
       <c r="H23" t="s">
-        <v>43</v>
+        <v>93</v>
       </c>
       <c r="I23" t="s">
-        <v>45</v>
+        <v>94</v>
       </c>
       <c r="J23" t="s">
-        <v>46</v>
+        <v>95</v>
       </c>
       <c r="K23" t="s">
-        <v>47</v>
+        <v>96</v>
       </c>
       <c r="L23" t="s">
-        <v>48</v>
+        <v>97</v>
       </c>
       <c r="M23" t="s">
-        <v>49</v>
+        <v>98</v>
       </c>
       <c r="N23" t="s">
-        <v>50</v>
+        <v>99</v>
+      </c>
+      <c r="O23" t="s">
+        <v>100</v>
+      </c>
+      <c r="P23" t="s">
+        <v>101</v>
+      </c>
+      <c r="Q23" t="s">
+        <v>102</v>
+      </c>
+      <c r="R23" t="s">
+        <v>103</v>
+      </c>
+      <c r="S23" t="s">
+        <v>104</v>
+      </c>
+      <c r="T23" t="s">
+        <v>105</v>
+      </c>
+      <c r="U23" t="s">
+        <v>106</v>
+      </c>
+      <c r="V23" t="s">
+        <v>107</v>
+      </c>
+      <c r="W23" t="s">
+        <v>108</v>
       </c>
     </row>
     <row r="24" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A24">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>70</v>
+        <v>40</v>
       </c>
       <c r="C24" t="s">
-        <v>71</v>
+        <v>41</v>
       </c>
       <c r="D24" t="s">
         <v>33</v>
@@ -2926,69 +2920,42 @@
         <v>33</v>
       </c>
       <c r="F24" t="s">
-        <v>72</v>
+        <v>42</v>
       </c>
       <c r="G24" t="s">
-        <v>73</v>
+        <v>109</v>
       </c>
       <c r="H24" t="s">
-        <v>74</v>
+        <v>43</v>
       </c>
       <c r="I24" t="s">
-        <v>75</v>
+        <v>45</v>
       </c>
       <c r="J24" t="s">
-        <v>76</v>
+        <v>46</v>
       </c>
       <c r="K24" t="s">
-        <v>77</v>
+        <v>47</v>
       </c>
       <c r="L24" t="s">
-        <v>78</v>
+        <v>48</v>
       </c>
       <c r="M24" t="s">
-        <v>79</v>
+        <v>49</v>
       </c>
       <c r="N24" t="s">
-        <v>80</v>
-      </c>
-      <c r="O24" t="s">
-        <v>81</v>
-      </c>
-      <c r="P24" t="s">
-        <v>82</v>
-      </c>
-      <c r="Q24" t="s">
-        <v>83</v>
-      </c>
-      <c r="R24" t="s">
-        <v>84</v>
-      </c>
-      <c r="S24" t="s">
-        <v>85</v>
-      </c>
-      <c r="T24" t="s">
-        <v>86</v>
-      </c>
-      <c r="U24" t="s">
-        <v>87</v>
-      </c>
-      <c r="V24" t="s">
-        <v>88</v>
-      </c>
-      <c r="W24" t="s">
-        <v>89</v>
+        <v>50</v>
       </c>
     </row>
     <row r="25" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A25">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>70</v>
       </c>
       <c r="C25" t="s">
-        <v>25</v>
+        <v>71</v>
       </c>
       <c r="D25" t="s">
         <v>33</v>
@@ -2997,54 +2964,69 @@
         <v>33</v>
       </c>
       <c r="F25" t="s">
-        <v>29</v>
+        <v>72</v>
       </c>
       <c r="G25" t="s">
-        <v>27</v>
+        <v>73</v>
       </c>
       <c r="H25" t="s">
-        <v>28</v>
+        <v>74</v>
       </c>
       <c r="I25" t="s">
-        <v>32</v>
+        <v>75</v>
       </c>
       <c r="J25" t="s">
-        <v>30</v>
+        <v>76</v>
       </c>
       <c r="K25" t="s">
-        <v>26</v>
+        <v>77</v>
       </c>
       <c r="L25" t="s">
-        <v>34</v>
+        <v>78</v>
       </c>
       <c r="M25" t="s">
-        <v>35</v>
+        <v>79</v>
       </c>
       <c r="N25" t="s">
-        <v>36</v>
+        <v>80</v>
       </c>
       <c r="O25" t="s">
-        <v>38</v>
+        <v>81</v>
       </c>
       <c r="P25" t="s">
-        <v>37</v>
+        <v>82</v>
       </c>
       <c r="Q25" t="s">
-        <v>31</v>
+        <v>83</v>
       </c>
       <c r="R25" t="s">
-        <v>39</v>
+        <v>84</v>
+      </c>
+      <c r="S25" t="s">
+        <v>85</v>
+      </c>
+      <c r="T25" t="s">
+        <v>86</v>
+      </c>
+      <c r="U25" t="s">
+        <v>87</v>
+      </c>
+      <c r="V25" t="s">
+        <v>88</v>
+      </c>
+      <c r="W25" t="s">
+        <v>89</v>
       </c>
     </row>
     <row r="26" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A26">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="B26" t="s">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="C26" t="s">
-        <v>41</v>
+        <v>25</v>
       </c>
       <c r="D26" t="s">
         <v>33</v>
@@ -3053,42 +3035,54 @@
         <v>33</v>
       </c>
       <c r="F26" t="s">
-        <v>42</v>
+        <v>29</v>
       </c>
       <c r="G26" t="s">
-        <v>44</v>
+        <v>27</v>
       </c>
       <c r="H26" t="s">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="I26" t="s">
-        <v>45</v>
+        <v>32</v>
       </c>
       <c r="J26" t="s">
-        <v>46</v>
+        <v>30</v>
       </c>
       <c r="K26" t="s">
-        <v>47</v>
+        <v>26</v>
       </c>
       <c r="L26" t="s">
-        <v>48</v>
+        <v>34</v>
       </c>
       <c r="M26" t="s">
-        <v>49</v>
+        <v>35</v>
       </c>
       <c r="N26" t="s">
-        <v>50</v>
+        <v>36</v>
+      </c>
+      <c r="O26" t="s">
+        <v>38</v>
+      </c>
+      <c r="P26" t="s">
+        <v>37</v>
+      </c>
+      <c r="Q26" t="s">
+        <v>31</v>
+      </c>
+      <c r="R26" t="s">
+        <v>39</v>
       </c>
     </row>
     <row r="27" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A27">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>51</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
-        <v>52</v>
+        <v>41</v>
       </c>
       <c r="D27" t="s">
         <v>33</v>
@@ -3097,66 +3091,42 @@
         <v>33</v>
       </c>
       <c r="F27" t="s">
-        <v>55</v>
+        <v>42</v>
       </c>
       <c r="G27" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
       <c r="H27" t="s">
-        <v>53</v>
+        <v>43</v>
       </c>
       <c r="I27" t="s">
-        <v>56</v>
+        <v>45</v>
       </c>
       <c r="J27" t="s">
-        <v>57</v>
+        <v>46</v>
       </c>
       <c r="K27" t="s">
-        <v>58</v>
+        <v>47</v>
       </c>
       <c r="L27" t="s">
-        <v>59</v>
+        <v>48</v>
       </c>
       <c r="M27" t="s">
-        <v>60</v>
+        <v>49</v>
       </c>
       <c r="N27" t="s">
-        <v>61</v>
-      </c>
-      <c r="O27" t="s">
-        <v>62</v>
-      </c>
-      <c r="P27" t="s">
-        <v>63</v>
-      </c>
-      <c r="Q27" t="s">
-        <v>64</v>
-      </c>
-      <c r="R27" t="s">
-        <v>65</v>
-      </c>
-      <c r="S27" t="s">
-        <v>66</v>
-      </c>
-      <c r="T27" t="s">
-        <v>67</v>
-      </c>
-      <c r="U27" t="s">
-        <v>68</v>
-      </c>
-      <c r="V27" t="s">
-        <v>69</v>
+        <v>50</v>
       </c>
     </row>
     <row r="28" spans="1:24" x14ac:dyDescent="0.25">
       <c r="A28">
-        <v>25</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
-        <v>365</v>
+        <v>51</v>
       </c>
       <c r="C28" t="s">
-        <v>345</v>
+        <v>52</v>
       </c>
       <c r="D28" t="s">
         <v>33</v>
@@ -3164,26 +3134,56 @@
       <c r="E28" t="s">
         <v>33</v>
       </c>
-      <c r="F28" s="4" t="s">
-        <v>366</v>
+      <c r="F28" t="s">
+        <v>55</v>
       </c>
       <c r="G28" t="s">
-        <v>367</v>
+        <v>54</v>
       </c>
       <c r="H28" t="s">
-        <v>368</v>
+        <v>53</v>
       </c>
       <c r="I28" t="s">
-        <v>371</v>
+        <v>56</v>
       </c>
       <c r="J28" t="s">
-        <v>369</v>
+        <v>57</v>
       </c>
       <c r="K28" t="s">
-        <v>370</v>
+        <v>58</v>
       </c>
       <c r="L28" t="s">
-        <v>360</v>
+        <v>59</v>
+      </c>
+      <c r="M28" t="s">
+        <v>60</v>
+      </c>
+      <c r="N28" t="s">
+        <v>61</v>
+      </c>
+      <c r="O28" t="s">
+        <v>62</v>
+      </c>
+      <c r="P28" t="s">
+        <v>63</v>
+      </c>
+      <c r="Q28" t="s">
+        <v>64</v>
+      </c>
+      <c r="R28" t="s">
+        <v>65</v>
+      </c>
+      <c r="S28" t="s">
+        <v>66</v>
+      </c>
+      <c r="T28" t="s">
+        <v>67</v>
+      </c>
+      <c r="U28" t="s">
+        <v>68</v>
+      </c>
+      <c r="V28" t="s">
+        <v>69</v>
       </c>
     </row>
   </sheetData>

</xml_diff>